<commit_message>
backend/server.js : update and trash feature
</commit_message>
<xml_diff>
--- a/backend/uploads/employees.xlsx
+++ b/backend/uploads/employees.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\CSVmaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEB989F0-C0D7-4537-A97C-6090ED2062DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5619BC41-80BD-4CA7-964C-E4A491E7BE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="150" windowWidth="18990" windowHeight="9930"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
@@ -22,157 +22,157 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>projectId</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>billability</t>
+  </si>
+  <si>
+    <t>Aaditya</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Aarya</t>
+  </si>
+  <si>
+    <t>Abhay</t>
+  </si>
+  <si>
+    <t>Abhijeet</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Abhinandan</t>
+  </si>
+  <si>
+    <t>Abhinay</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Abimanyu</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>Akshat</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Avi</t>
+  </si>
+  <si>
+    <t>Balaraam</t>
+  </si>
+  <si>
+    <t>Bharat</t>
+  </si>
+  <si>
+    <t>Bhaskar</t>
+  </si>
+  <si>
+    <t>Bhaumik</t>
+  </si>
+  <si>
+    <t>Bijay</t>
+  </si>
+  <si>
+    <t>Brijesh</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Chandan</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Chirag</t>
+  </si>
+  <si>
+    <t>Chiranjeeve</t>
+  </si>
+  <si>
+    <t>Daksh</t>
+  </si>
+  <si>
+    <t>Daman</t>
+  </si>
+  <si>
+    <t>Depen</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Dhruv</t>
+  </si>
+  <si>
+    <t>Divyanshu</t>
+  </si>
+  <si>
+    <t>Ekambar</t>
+  </si>
+  <si>
+    <t>Ekansh</t>
+  </si>
+  <si>
+    <t>Ekaraj</t>
+  </si>
+  <si>
+    <t>Eklavya</t>
+  </si>
+  <si>
+    <t>Elilarasan</t>
+  </si>
+  <si>
+    <t>Falak</t>
+  </si>
+  <si>
+    <t>Gagan</t>
+  </si>
+  <si>
+    <t>Gajendra</t>
+  </si>
+  <si>
     <t>empId</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>projectId</t>
-  </si>
-  <si>
-    <t>grade</t>
-  </si>
-  <si>
-    <t>billability</t>
-  </si>
-  <si>
-    <t>Aaditya</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Aarya</t>
-  </si>
-  <si>
-    <t>Abhay</t>
-  </si>
-  <si>
-    <t>Abhijeet</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Abhinandan</t>
-  </si>
-  <si>
-    <t>Abhinay</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
-    <t>Abimanyu</t>
-  </si>
-  <si>
-    <t>Aditya</t>
-  </si>
-  <si>
-    <t>Akhil</t>
-  </si>
-  <si>
-    <t>Akshat</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Anil</t>
-  </si>
-  <si>
-    <t>Avi</t>
-  </si>
-  <si>
-    <t>Balaraam</t>
-  </si>
-  <si>
-    <t>Bharat</t>
-  </si>
-  <si>
-    <t>Bhaskar</t>
-  </si>
-  <si>
-    <t>Bhaumik</t>
-  </si>
-  <si>
-    <t>Bijay</t>
-  </si>
-  <si>
-    <t>Brijesh</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Chandan</t>
-  </si>
-  <si>
-    <t>Chetan</t>
-  </si>
-  <si>
-    <t>Chirag</t>
-  </si>
-  <si>
-    <t>Chiranjeeve</t>
-  </si>
-  <si>
-    <t>Daksh</t>
-  </si>
-  <si>
-    <t>Daman</t>
-  </si>
-  <si>
-    <t>Depen</t>
-  </si>
-  <si>
-    <t>Dev</t>
-  </si>
-  <si>
-    <t>Dhruv</t>
-  </si>
-  <si>
-    <t>Divyanshu</t>
-  </si>
-  <si>
-    <t>Ekambar</t>
-  </si>
-  <si>
-    <t>Ekansh</t>
-  </si>
-  <si>
-    <t>Ekaraj</t>
-  </si>
-  <si>
-    <t>Eklavya</t>
-  </si>
-  <si>
-    <t>Elilarasan</t>
-  </si>
-  <si>
-    <t>Falak</t>
-  </si>
-  <si>
-    <t>Gagan</t>
-  </si>
-  <si>
-    <t>Gajendra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1015,19 +1015,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1035,16 +1035,16 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>4823</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1052,16 +1052,16 @@
         <v>2000</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>5830</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1069,16 +1069,16 @@
         <v>3000</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>5830</v>
       </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1086,16 +1086,16 @@
         <v>4000</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>5830</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1103,16 +1103,16 @@
         <v>5000</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>3561</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1120,16 +1120,16 @@
         <v>6000</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>5830</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1137,16 +1137,16 @@
         <v>7000</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>2319</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1154,16 +1154,16 @@
         <v>8000</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>3561</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1171,16 +1171,16 @@
         <v>9000</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>9176</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1188,16 +1188,16 @@
         <v>1000</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>1247</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1205,16 +1205,16 @@
         <v>1100</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>1247</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1222,16 +1222,16 @@
         <v>1200</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>3561</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1239,16 +1239,16 @@
         <v>1300</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>6908</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1256,16 +1256,16 @@
         <v>1400</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>1247</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1273,16 +1273,16 @@
         <v>1500</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>3561</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1290,16 +1290,16 @@
         <v>1600</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>1247</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1307,16 +1307,16 @@
         <v>1700</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>9176</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1324,16 +1324,16 @@
         <v>1800</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>1247</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1341,16 +1341,16 @@
         <v>1900</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>1247</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1358,16 +1358,16 @@
         <v>2000</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>6908</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1375,16 +1375,16 @@
         <v>2100</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <v>3561</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1392,16 +1392,16 @@
         <v>2200</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>4823</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1409,16 +1409,16 @@
         <v>2300</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>2319</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1426,16 +1426,16 @@
         <v>2400</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>3561</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1443,16 +1443,16 @@
         <v>2500</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>5830</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1460,16 +1460,16 @@
         <v>2600</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <v>3561</v>
       </c>
       <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
         <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1477,16 +1477,16 @@
         <v>2700</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>5830</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1494,16 +1494,16 @@
         <v>2800</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29">
         <v>2319</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1511,16 +1511,16 @@
         <v>2900</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30">
         <v>2319</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1528,16 +1528,16 @@
         <v>3000</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>3561</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1545,16 +1545,16 @@
         <v>3100</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>3561</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1562,16 +1562,16 @@
         <v>3200</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33">
         <v>1247</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1579,16 +1579,16 @@
         <v>3300</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>1247</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1596,16 +1596,16 @@
         <v>3400</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35">
         <v>9176</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1613,16 +1613,16 @@
         <v>3500</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36">
         <v>1247</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1630,16 +1630,16 @@
         <v>3600</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37">
         <v>2319</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1647,16 +1647,16 @@
         <v>3700</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38">
         <v>2319</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>